<commit_message>
Toma bien los numeros
</commit_message>
<xml_diff>
--- a/script_DNRPA/prueba.xlsx
+++ b/script_DNRPA/prueba.xlsx
@@ -390,14 +390,1213 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Provincia / Mes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>BUENOS AIRES</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>C.AUTONOMA DE BS.AS</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>CATAMARCA</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>CORDOBA</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>CORRIENTES</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>CHACO</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>CHUBUT</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>ENTRE RIOS</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>FORMOSA</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>JUJUY</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>LA PAMPA</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>LA RIOJA</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>MENDOZA</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>MISIONES</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>NEUQUEN</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>RIO NEGRO</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>SALTA</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>SAN JUAN</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>SAN LUIS</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>SANTA CRUZ</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>SANTA FE</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>SGO.DEL ESTERO</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>TUCUMAN</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>T.DEL FUEGO</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ene</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>35306</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15737</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1036</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10692</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2796</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2299</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2167</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3373</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1192</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1562</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1213</v>
+      </c>
+      <c r="M2" t="n">
+        <v>827</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4211</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2105</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2344</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1537</v>
+      </c>
+      <c r="R2" t="n">
+        <v>2546</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1326</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1107</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1439</v>
+      </c>
+      <c r="V2" t="n">
+        <v>9712</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1386</v>
+      </c>
+      <c r="X2" t="n">
+        <v>2781</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>819</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>109513</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>19362</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9521</v>
+      </c>
+      <c r="D3" t="n">
+        <v>426</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5474</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1360</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1101</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1392</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1427</v>
+      </c>
+      <c r="J3" t="n">
+        <v>622</v>
+      </c>
+      <c r="K3" t="n">
+        <v>902</v>
+      </c>
+      <c r="L3" t="n">
+        <v>605</v>
+      </c>
+      <c r="M3" t="n">
+        <v>375</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2445</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1009</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1360</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>951</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1173</v>
+      </c>
+      <c r="S3" t="n">
+        <v>588</v>
+      </c>
+      <c r="T3" t="n">
+        <v>566</v>
+      </c>
+      <c r="U3" t="n">
+        <v>866</v>
+      </c>
+      <c r="V3" t="n">
+        <v>4677</v>
+      </c>
+      <c r="W3" t="n">
+        <v>706</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1371</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>651</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>58930</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>16892</v>
+      </c>
+      <c r="C4" t="n">
+        <v>8638</v>
+      </c>
+      <c r="D4" t="n">
+        <v>429</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5103</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1105</v>
+      </c>
+      <c r="G4" t="n">
+        <v>822</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1217</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1405</v>
+      </c>
+      <c r="J4" t="n">
+        <v>494</v>
+      </c>
+      <c r="K4" t="n">
+        <v>755</v>
+      </c>
+      <c r="L4" t="n">
+        <v>553</v>
+      </c>
+      <c r="M4" t="n">
+        <v>338</v>
+      </c>
+      <c r="N4" t="n">
+        <v>2077</v>
+      </c>
+      <c r="O4" t="n">
+        <v>868</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1207</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>807</v>
+      </c>
+      <c r="R4" t="n">
+        <v>1123</v>
+      </c>
+      <c r="S4" t="n">
+        <v>647</v>
+      </c>
+      <c r="T4" t="n">
+        <v>458</v>
+      </c>
+      <c r="U4" t="n">
+        <v>712</v>
+      </c>
+      <c r="V4" t="n">
+        <v>3910</v>
+      </c>
+      <c r="W4" t="n">
+        <v>528</v>
+      </c>
+      <c r="X4" t="n">
+        <v>1226</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>564</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>51878</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Abr</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17525</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8369</v>
+      </c>
+      <c r="D5" t="n">
+        <v>414</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5335</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1214</v>
+      </c>
+      <c r="G5" t="n">
+        <v>934</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1108</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1435</v>
+      </c>
+      <c r="J5" t="n">
+        <v>575</v>
+      </c>
+      <c r="K5" t="n">
+        <v>774</v>
+      </c>
+      <c r="L5" t="n">
+        <v>548</v>
+      </c>
+      <c r="M5" t="n">
+        <v>339</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2036</v>
+      </c>
+      <c r="O5" t="n">
+        <v>837</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1384</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>875</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1084</v>
+      </c>
+      <c r="S5" t="n">
+        <v>617</v>
+      </c>
+      <c r="T5" t="n">
+        <v>515</v>
+      </c>
+      <c r="U5" t="n">
+        <v>850</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4222</v>
+      </c>
+      <c r="W5" t="n">
+        <v>721</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1421</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>650</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>53782</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>18310</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9189</v>
+      </c>
+      <c r="D6" t="n">
+        <v>498</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5526</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1344</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1005</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1290</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1516</v>
+      </c>
+      <c r="J6" t="n">
+        <v>555</v>
+      </c>
+      <c r="K6" t="n">
+        <v>825</v>
+      </c>
+      <c r="L6" t="n">
+        <v>565</v>
+      </c>
+      <c r="M6" t="n">
+        <v>366</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2210</v>
+      </c>
+      <c r="O6" t="n">
+        <v>900</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1474</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>942</v>
+      </c>
+      <c r="R6" t="n">
+        <v>1139</v>
+      </c>
+      <c r="S6" t="n">
+        <v>612</v>
+      </c>
+      <c r="T6" t="n">
+        <v>549</v>
+      </c>
+      <c r="U6" t="n">
+        <v>886</v>
+      </c>
+      <c r="V6" t="n">
+        <v>4587</v>
+      </c>
+      <c r="W6" t="n">
+        <v>587</v>
+      </c>
+      <c r="X6" t="n">
+        <v>1357</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>589</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>56821</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>16704</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8687</v>
+      </c>
+      <c r="D7" t="n">
+        <v>451</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5470</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1298</v>
+      </c>
+      <c r="G7" t="n">
+        <v>963</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1294</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1512</v>
+      </c>
+      <c r="J7" t="n">
+        <v>555</v>
+      </c>
+      <c r="K7" t="n">
+        <v>702</v>
+      </c>
+      <c r="L7" t="n">
+        <v>558</v>
+      </c>
+      <c r="M7" t="n">
+        <v>337</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2092</v>
+      </c>
+      <c r="O7" t="n">
+        <v>898</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1352</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>853</v>
+      </c>
+      <c r="R7" t="n">
+        <v>1086</v>
+      </c>
+      <c r="S7" t="n">
+        <v>579</v>
+      </c>
+      <c r="T7" t="n">
+        <v>455</v>
+      </c>
+      <c r="U7" t="n">
+        <v>798</v>
+      </c>
+      <c r="V7" t="n">
+        <v>4429</v>
+      </c>
+      <c r="W7" t="n">
+        <v>604</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1354</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>485</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>53516</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>19624</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9577</v>
+      </c>
+      <c r="D8" t="n">
+        <v>535</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6517</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1269</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1142</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1458</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1660</v>
+      </c>
+      <c r="J8" t="n">
+        <v>553</v>
+      </c>
+      <c r="K8" t="n">
+        <v>777</v>
+      </c>
+      <c r="L8" t="n">
+        <v>623</v>
+      </c>
+      <c r="M8" t="n">
+        <v>329</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2361</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1131</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1572</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1035</v>
+      </c>
+      <c r="R8" t="n">
+        <v>1367</v>
+      </c>
+      <c r="S8" t="n">
+        <v>757</v>
+      </c>
+      <c r="T8" t="n">
+        <v>536</v>
+      </c>
+      <c r="U8" t="n">
+        <v>934</v>
+      </c>
+      <c r="V8" t="n">
+        <v>5085</v>
+      </c>
+      <c r="W8" t="n">
+        <v>700</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1511</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>614</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>61667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ago</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>18820</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8805</v>
+      </c>
+      <c r="D9" t="n">
+        <v>477</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5795</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1249</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1114</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1355</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1604</v>
+      </c>
+      <c r="J9" t="n">
+        <v>506</v>
+      </c>
+      <c r="K9" t="n">
+        <v>769</v>
+      </c>
+      <c r="L9" t="n">
+        <v>557</v>
+      </c>
+      <c r="M9" t="n">
+        <v>409</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2564</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1068</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1375</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>975</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1236</v>
+      </c>
+      <c r="S9" t="n">
+        <v>657</v>
+      </c>
+      <c r="T9" t="n">
+        <v>457</v>
+      </c>
+      <c r="U9" t="n">
+        <v>901</v>
+      </c>
+      <c r="V9" t="n">
+        <v>5057</v>
+      </c>
+      <c r="W9" t="n">
+        <v>695</v>
+      </c>
+      <c r="X9" t="n">
+        <v>1501</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>608</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>58554</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>18495</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9712</v>
+      </c>
+      <c r="D10" t="n">
+        <v>517</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5840</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1264</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1148</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1382</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1618</v>
+      </c>
+      <c r="J10" t="n">
+        <v>525</v>
+      </c>
+      <c r="K10" t="n">
+        <v>714</v>
+      </c>
+      <c r="L10" t="n">
+        <v>614</v>
+      </c>
+      <c r="M10" t="n">
+        <v>349</v>
+      </c>
+      <c r="N10" t="n">
+        <v>2549</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1097</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1445</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>903</v>
+      </c>
+      <c r="R10" t="n">
+        <v>1258</v>
+      </c>
+      <c r="S10" t="n">
+        <v>660</v>
+      </c>
+      <c r="T10" t="n">
+        <v>512</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1007</v>
+      </c>
+      <c r="V10" t="n">
+        <v>5173</v>
+      </c>
+      <c r="W10" t="n">
+        <v>676</v>
+      </c>
+      <c r="X10" t="n">
+        <v>1433</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>806</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>59697</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>17118</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8826</v>
+      </c>
+      <c r="D11" t="n">
+        <v>439</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5271</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1178</v>
+      </c>
+      <c r="G11" t="n">
+        <v>998</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1226</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1420</v>
+      </c>
+      <c r="J11" t="n">
+        <v>506</v>
+      </c>
+      <c r="K11" t="n">
+        <v>626</v>
+      </c>
+      <c r="L11" t="n">
+        <v>519</v>
+      </c>
+      <c r="M11" t="n">
+        <v>323</v>
+      </c>
+      <c r="N11" t="n">
+        <v>2232</v>
+      </c>
+      <c r="O11" t="n">
+        <v>965</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1472</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>868</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1207</v>
+      </c>
+      <c r="S11" t="n">
+        <v>640</v>
+      </c>
+      <c r="T11" t="n">
+        <v>493</v>
+      </c>
+      <c r="U11" t="n">
+        <v>958</v>
+      </c>
+      <c r="V11" t="n">
+        <v>4627</v>
+      </c>
+      <c r="W11" t="n">
+        <v>597</v>
+      </c>
+      <c r="X11" t="n">
+        <v>1437</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>753</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>54699</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>12187</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6905</v>
+      </c>
+      <c r="D12" t="n">
+        <v>287</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3818</v>
+      </c>
+      <c r="F12" t="n">
+        <v>816</v>
+      </c>
+      <c r="G12" t="n">
+        <v>795</v>
+      </c>
+      <c r="H12" t="n">
+        <v>919</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1050</v>
+      </c>
+      <c r="J12" t="n">
+        <v>402</v>
+      </c>
+      <c r="K12" t="n">
+        <v>541</v>
+      </c>
+      <c r="L12" t="n">
+        <v>375</v>
+      </c>
+      <c r="M12" t="n">
+        <v>187</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1541</v>
+      </c>
+      <c r="O12" t="n">
+        <v>721</v>
+      </c>
+      <c r="P12" t="n">
+        <v>1071</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>677</v>
+      </c>
+      <c r="R12" t="n">
+        <v>892</v>
+      </c>
+      <c r="S12" t="n">
+        <v>398</v>
+      </c>
+      <c r="T12" t="n">
+        <v>351</v>
+      </c>
+      <c r="U12" t="n">
+        <v>712</v>
+      </c>
+      <c r="V12" t="n">
+        <v>3307</v>
+      </c>
+      <c r="W12" t="n">
+        <v>437</v>
+      </c>
+      <c r="X12" t="n">
+        <v>1111</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>568</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>40068</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dic</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9367</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5843</v>
+      </c>
+      <c r="D13" t="n">
+        <v>224</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2772</v>
+      </c>
+      <c r="F13" t="n">
+        <v>584</v>
+      </c>
+      <c r="G13" t="n">
+        <v>528</v>
+      </c>
+      <c r="H13" t="n">
+        <v>825</v>
+      </c>
+      <c r="I13" t="n">
+        <v>743</v>
+      </c>
+      <c r="J13" t="n">
+        <v>251</v>
+      </c>
+      <c r="K13" t="n">
+        <v>398</v>
+      </c>
+      <c r="L13" t="n">
+        <v>271</v>
+      </c>
+      <c r="M13" t="n">
+        <v>122</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1068</v>
+      </c>
+      <c r="O13" t="n">
+        <v>443</v>
+      </c>
+      <c r="P13" t="n">
+        <v>847</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>532</v>
+      </c>
+      <c r="R13" t="n">
+        <v>781</v>
+      </c>
+      <c r="S13" t="n">
+        <v>253</v>
+      </c>
+      <c r="T13" t="n">
+        <v>253</v>
+      </c>
+      <c r="U13" t="n">
+        <v>584</v>
+      </c>
+      <c r="V13" t="n">
+        <v>2343</v>
+      </c>
+      <c r="W13" t="n">
+        <v>255</v>
+      </c>
+      <c r="X13" t="n">
+        <v>680</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>503</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>30470</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>219710</v>
+      </c>
+      <c r="C14" t="n">
+        <v>109809</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5733</v>
+      </c>
+      <c r="E14" t="n">
+        <v>67613</v>
+      </c>
+      <c r="F14" t="n">
+        <v>15477</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12849</v>
+      </c>
+      <c r="H14" t="n">
+        <v>15633</v>
+      </c>
+      <c r="I14" t="n">
+        <v>18763</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6736</v>
+      </c>
+      <c r="K14" t="n">
+        <v>9345</v>
+      </c>
+      <c r="L14" t="n">
+        <v>7001</v>
+      </c>
+      <c r="M14" t="n">
+        <v>4301</v>
+      </c>
+      <c r="N14" t="n">
+        <v>27386</v>
+      </c>
+      <c r="O14" t="n">
+        <v>12042</v>
+      </c>
+      <c r="P14" t="n">
+        <v>16903</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>10955</v>
+      </c>
+      <c r="R14" t="n">
+        <v>14892</v>
+      </c>
+      <c r="S14" t="n">
+        <v>7734</v>
+      </c>
+      <c r="T14" t="n">
+        <v>6252</v>
+      </c>
+      <c r="U14" t="n">
+        <v>10647</v>
+      </c>
+      <c r="V14" t="n">
+        <v>57129</v>
+      </c>
+      <c r="W14" t="n">
+        <v>7892</v>
+      </c>
+      <c r="X14" t="n">
+        <v>17183</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>7610</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>689595</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tabla sin total y numeros corregidos
</commit_message>
<xml_diff>
--- a/script_DNRPA/prueba.xlsx
+++ b/script_DNRPA/prueba.xlsx
@@ -16,12 +16,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -45,8 +53,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,13 +399,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.140625" customWidth="1" style="1" min="1" max="16384"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -1514,89 +1526,8 @@
         <v>30470</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>219710</v>
-      </c>
-      <c r="C14" t="n">
-        <v>109809</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5733</v>
-      </c>
-      <c r="E14" t="n">
-        <v>67613</v>
-      </c>
-      <c r="F14" t="n">
-        <v>15477</v>
-      </c>
-      <c r="G14" t="n">
-        <v>12849</v>
-      </c>
-      <c r="H14" t="n">
-        <v>15633</v>
-      </c>
-      <c r="I14" t="n">
-        <v>18763</v>
-      </c>
-      <c r="J14" t="n">
-        <v>6736</v>
-      </c>
-      <c r="K14" t="n">
-        <v>9345</v>
-      </c>
-      <c r="L14" t="n">
-        <v>7001</v>
-      </c>
-      <c r="M14" t="n">
-        <v>4301</v>
-      </c>
-      <c r="N14" t="n">
-        <v>27386</v>
-      </c>
-      <c r="O14" t="n">
-        <v>12042</v>
-      </c>
-      <c r="P14" t="n">
-        <v>16903</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>10955</v>
-      </c>
-      <c r="R14" t="n">
-        <v>14892</v>
-      </c>
-      <c r="S14" t="n">
-        <v>7734</v>
-      </c>
-      <c r="T14" t="n">
-        <v>6252</v>
-      </c>
-      <c r="U14" t="n">
-        <v>10647</v>
-      </c>
-      <c r="V14" t="n">
-        <v>57129</v>
-      </c>
-      <c r="W14" t="n">
-        <v>7892</v>
-      </c>
-      <c r="X14" t="n">
-        <v>17183</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>7610</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>689595</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
carga la tabla, pero no el update
</commit_message>
<xml_diff>
--- a/script_DNRPA/prueba.xlsx
+++ b/script_DNRPA/prueba.xlsx
@@ -402,7 +402,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O25" sqref="O25"/>
@@ -546,10 +546,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2014-01-01</t>
-        </is>
+      <c r="A2" s="2" t="n">
+        <v>41640</v>
       </c>
       <c r="B2" t="n">
         <v>35306</v>
@@ -628,10 +626,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2014-02-01</t>
-        </is>
+      <c r="A3" s="2" t="n">
+        <v>41671</v>
       </c>
       <c r="B3" t="n">
         <v>19362</v>
@@ -710,10 +706,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2014-03-01</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>41699</v>
       </c>
       <c r="B4" t="n">
         <v>16892</v>
@@ -792,10 +786,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2014-04-01</t>
-        </is>
+      <c r="A5" s="2" t="n">
+        <v>41730</v>
       </c>
       <c r="B5" t="n">
         <v>17525</v>
@@ -874,10 +866,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2014-05-01</t>
-        </is>
+      <c r="A6" s="2" t="n">
+        <v>41760</v>
       </c>
       <c r="B6" t="n">
         <v>18310</v>
@@ -956,10 +946,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2014-06-01</t>
-        </is>
+      <c r="A7" s="2" t="n">
+        <v>41791</v>
       </c>
       <c r="B7" t="n">
         <v>16704</v>
@@ -1038,10 +1026,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2014-07-01</t>
-        </is>
+      <c r="A8" s="2" t="n">
+        <v>41821</v>
       </c>
       <c r="B8" t="n">
         <v>19624</v>
@@ -1120,10 +1106,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2014-08-01</t>
-        </is>
+      <c r="A9" s="2" t="n">
+        <v>41852</v>
       </c>
       <c r="B9" t="n">
         <v>18820</v>
@@ -1202,10 +1186,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2014-09-01</t>
-        </is>
+      <c r="A10" s="2" t="n">
+        <v>41883</v>
       </c>
       <c r="B10" t="n">
         <v>18495</v>
@@ -1284,10 +1266,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2014-10-01</t>
-        </is>
+      <c r="A11" s="2" t="n">
+        <v>41913</v>
       </c>
       <c r="B11" t="n">
         <v>17118</v>
@@ -1366,10 +1346,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2014-11-01</t>
-        </is>
+      <c r="A12" s="2" t="n">
+        <v>41944</v>
       </c>
       <c r="B12" t="n">
         <v>12187</v>
@@ -1448,10 +1426,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2014-12-01</t>
-        </is>
+      <c r="A13" s="2" t="n">
+        <v>41974</v>
       </c>
       <c r="B13" t="n">
         <v>9367</v>
@@ -1526,1098 +1502,6 @@
         <v>503</v>
       </c>
       <c r="Z13" t="n">
-        <v>30470</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Provincia / Mes</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>BUENOS AIRES</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>C.AUTONOMA DE BS.AS</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>CATAMARCA</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>CORDOBA</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>CORRIENTES</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>CHACO</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>CHUBUT</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>ENTRE RIOS</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>FORMOSA</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>JUJUY</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>LA PAMPA</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>LA RIOJA</t>
-        </is>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>MENDOZA</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>MISIONES</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>NEUQUEN</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>RIO NEGRO</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>SALTA</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>SAN JUAN</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>SAN LUIS</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>SANTA CRUZ</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>SANTA FE</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>SGO.DEL ESTERO</t>
-        </is>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>TUCUMAN</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>T.DEL FUEGO</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>41640</v>
-      </c>
-      <c r="B15" t="n">
-        <v>35306</v>
-      </c>
-      <c r="C15" t="n">
-        <v>15737</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1036</v>
-      </c>
-      <c r="E15" t="n">
-        <v>10692</v>
-      </c>
-      <c r="F15" t="n">
-        <v>2796</v>
-      </c>
-      <c r="G15" t="n">
-        <v>2299</v>
-      </c>
-      <c r="H15" t="n">
-        <v>2167</v>
-      </c>
-      <c r="I15" t="n">
-        <v>3373</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1192</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1562</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1213</v>
-      </c>
-      <c r="M15" t="n">
-        <v>827</v>
-      </c>
-      <c r="N15" t="n">
-        <v>4211</v>
-      </c>
-      <c r="O15" t="n">
-        <v>2105</v>
-      </c>
-      <c r="P15" t="n">
-        <v>2344</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>1537</v>
-      </c>
-      <c r="R15" t="n">
-        <v>2546</v>
-      </c>
-      <c r="S15" t="n">
-        <v>1326</v>
-      </c>
-      <c r="T15" t="n">
-        <v>1107</v>
-      </c>
-      <c r="U15" t="n">
-        <v>1439</v>
-      </c>
-      <c r="V15" t="n">
-        <v>9712</v>
-      </c>
-      <c r="W15" t="n">
-        <v>1386</v>
-      </c>
-      <c r="X15" t="n">
-        <v>2781</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>819</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>109513</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>41671</v>
-      </c>
-      <c r="B16" t="n">
-        <v>19362</v>
-      </c>
-      <c r="C16" t="n">
-        <v>9521</v>
-      </c>
-      <c r="D16" t="n">
-        <v>426</v>
-      </c>
-      <c r="E16" t="n">
-        <v>5474</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1360</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1101</v>
-      </c>
-      <c r="H16" t="n">
-        <v>1392</v>
-      </c>
-      <c r="I16" t="n">
-        <v>1427</v>
-      </c>
-      <c r="J16" t="n">
-        <v>622</v>
-      </c>
-      <c r="K16" t="n">
-        <v>902</v>
-      </c>
-      <c r="L16" t="n">
-        <v>605</v>
-      </c>
-      <c r="M16" t="n">
-        <v>375</v>
-      </c>
-      <c r="N16" t="n">
-        <v>2445</v>
-      </c>
-      <c r="O16" t="n">
-        <v>1009</v>
-      </c>
-      <c r="P16" t="n">
-        <v>1360</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>951</v>
-      </c>
-      <c r="R16" t="n">
-        <v>1173</v>
-      </c>
-      <c r="S16" t="n">
-        <v>588</v>
-      </c>
-      <c r="T16" t="n">
-        <v>566</v>
-      </c>
-      <c r="U16" t="n">
-        <v>866</v>
-      </c>
-      <c r="V16" t="n">
-        <v>4677</v>
-      </c>
-      <c r="W16" t="n">
-        <v>706</v>
-      </c>
-      <c r="X16" t="n">
-        <v>1371</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>651</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>58930</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>41699</v>
-      </c>
-      <c r="B17" t="n">
-        <v>16892</v>
-      </c>
-      <c r="C17" t="n">
-        <v>8638</v>
-      </c>
-      <c r="D17" t="n">
-        <v>429</v>
-      </c>
-      <c r="E17" t="n">
-        <v>5103</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1105</v>
-      </c>
-      <c r="G17" t="n">
-        <v>822</v>
-      </c>
-      <c r="H17" t="n">
-        <v>1217</v>
-      </c>
-      <c r="I17" t="n">
-        <v>1405</v>
-      </c>
-      <c r="J17" t="n">
-        <v>494</v>
-      </c>
-      <c r="K17" t="n">
-        <v>755</v>
-      </c>
-      <c r="L17" t="n">
-        <v>553</v>
-      </c>
-      <c r="M17" t="n">
-        <v>338</v>
-      </c>
-      <c r="N17" t="n">
-        <v>2077</v>
-      </c>
-      <c r="O17" t="n">
-        <v>868</v>
-      </c>
-      <c r="P17" t="n">
-        <v>1207</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>807</v>
-      </c>
-      <c r="R17" t="n">
-        <v>1123</v>
-      </c>
-      <c r="S17" t="n">
-        <v>647</v>
-      </c>
-      <c r="T17" t="n">
-        <v>458</v>
-      </c>
-      <c r="U17" t="n">
-        <v>712</v>
-      </c>
-      <c r="V17" t="n">
-        <v>3910</v>
-      </c>
-      <c r="W17" t="n">
-        <v>528</v>
-      </c>
-      <c r="X17" t="n">
-        <v>1226</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>564</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>51878</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>41730</v>
-      </c>
-      <c r="B18" t="n">
-        <v>17525</v>
-      </c>
-      <c r="C18" t="n">
-        <v>8369</v>
-      </c>
-      <c r="D18" t="n">
-        <v>414</v>
-      </c>
-      <c r="E18" t="n">
-        <v>5335</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1214</v>
-      </c>
-      <c r="G18" t="n">
-        <v>934</v>
-      </c>
-      <c r="H18" t="n">
-        <v>1108</v>
-      </c>
-      <c r="I18" t="n">
-        <v>1435</v>
-      </c>
-      <c r="J18" t="n">
-        <v>575</v>
-      </c>
-      <c r="K18" t="n">
-        <v>774</v>
-      </c>
-      <c r="L18" t="n">
-        <v>548</v>
-      </c>
-      <c r="M18" t="n">
-        <v>339</v>
-      </c>
-      <c r="N18" t="n">
-        <v>2036</v>
-      </c>
-      <c r="O18" t="n">
-        <v>837</v>
-      </c>
-      <c r="P18" t="n">
-        <v>1384</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>875</v>
-      </c>
-      <c r="R18" t="n">
-        <v>1084</v>
-      </c>
-      <c r="S18" t="n">
-        <v>617</v>
-      </c>
-      <c r="T18" t="n">
-        <v>515</v>
-      </c>
-      <c r="U18" t="n">
-        <v>850</v>
-      </c>
-      <c r="V18" t="n">
-        <v>4222</v>
-      </c>
-      <c r="W18" t="n">
-        <v>721</v>
-      </c>
-      <c r="X18" t="n">
-        <v>1421</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>650</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>53782</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>41760</v>
-      </c>
-      <c r="B19" t="n">
-        <v>18310</v>
-      </c>
-      <c r="C19" t="n">
-        <v>9189</v>
-      </c>
-      <c r="D19" t="n">
-        <v>498</v>
-      </c>
-      <c r="E19" t="n">
-        <v>5526</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1344</v>
-      </c>
-      <c r="G19" t="n">
-        <v>1005</v>
-      </c>
-      <c r="H19" t="n">
-        <v>1290</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1516</v>
-      </c>
-      <c r="J19" t="n">
-        <v>555</v>
-      </c>
-      <c r="K19" t="n">
-        <v>825</v>
-      </c>
-      <c r="L19" t="n">
-        <v>565</v>
-      </c>
-      <c r="M19" t="n">
-        <v>366</v>
-      </c>
-      <c r="N19" t="n">
-        <v>2210</v>
-      </c>
-      <c r="O19" t="n">
-        <v>900</v>
-      </c>
-      <c r="P19" t="n">
-        <v>1474</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>942</v>
-      </c>
-      <c r="R19" t="n">
-        <v>1139</v>
-      </c>
-      <c r="S19" t="n">
-        <v>612</v>
-      </c>
-      <c r="T19" t="n">
-        <v>549</v>
-      </c>
-      <c r="U19" t="n">
-        <v>886</v>
-      </c>
-      <c r="V19" t="n">
-        <v>4587</v>
-      </c>
-      <c r="W19" t="n">
-        <v>587</v>
-      </c>
-      <c r="X19" t="n">
-        <v>1357</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>589</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>56821</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>41791</v>
-      </c>
-      <c r="B20" t="n">
-        <v>16704</v>
-      </c>
-      <c r="C20" t="n">
-        <v>8687</v>
-      </c>
-      <c r="D20" t="n">
-        <v>451</v>
-      </c>
-      <c r="E20" t="n">
-        <v>5470</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1298</v>
-      </c>
-      <c r="G20" t="n">
-        <v>963</v>
-      </c>
-      <c r="H20" t="n">
-        <v>1294</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1512</v>
-      </c>
-      <c r="J20" t="n">
-        <v>555</v>
-      </c>
-      <c r="K20" t="n">
-        <v>702</v>
-      </c>
-      <c r="L20" t="n">
-        <v>558</v>
-      </c>
-      <c r="M20" t="n">
-        <v>337</v>
-      </c>
-      <c r="N20" t="n">
-        <v>2092</v>
-      </c>
-      <c r="O20" t="n">
-        <v>898</v>
-      </c>
-      <c r="P20" t="n">
-        <v>1352</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>853</v>
-      </c>
-      <c r="R20" t="n">
-        <v>1086</v>
-      </c>
-      <c r="S20" t="n">
-        <v>579</v>
-      </c>
-      <c r="T20" t="n">
-        <v>455</v>
-      </c>
-      <c r="U20" t="n">
-        <v>798</v>
-      </c>
-      <c r="V20" t="n">
-        <v>4429</v>
-      </c>
-      <c r="W20" t="n">
-        <v>604</v>
-      </c>
-      <c r="X20" t="n">
-        <v>1354</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>485</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>53516</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>41821</v>
-      </c>
-      <c r="B21" t="n">
-        <v>19624</v>
-      </c>
-      <c r="C21" t="n">
-        <v>9577</v>
-      </c>
-      <c r="D21" t="n">
-        <v>535</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6517</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1269</v>
-      </c>
-      <c r="G21" t="n">
-        <v>1142</v>
-      </c>
-      <c r="H21" t="n">
-        <v>1458</v>
-      </c>
-      <c r="I21" t="n">
-        <v>1660</v>
-      </c>
-      <c r="J21" t="n">
-        <v>553</v>
-      </c>
-      <c r="K21" t="n">
-        <v>777</v>
-      </c>
-      <c r="L21" t="n">
-        <v>623</v>
-      </c>
-      <c r="M21" t="n">
-        <v>329</v>
-      </c>
-      <c r="N21" t="n">
-        <v>2361</v>
-      </c>
-      <c r="O21" t="n">
-        <v>1131</v>
-      </c>
-      <c r="P21" t="n">
-        <v>1572</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>1035</v>
-      </c>
-      <c r="R21" t="n">
-        <v>1367</v>
-      </c>
-      <c r="S21" t="n">
-        <v>757</v>
-      </c>
-      <c r="T21" t="n">
-        <v>536</v>
-      </c>
-      <c r="U21" t="n">
-        <v>934</v>
-      </c>
-      <c r="V21" t="n">
-        <v>5085</v>
-      </c>
-      <c r="W21" t="n">
-        <v>700</v>
-      </c>
-      <c r="X21" t="n">
-        <v>1511</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>614</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>61667</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>41852</v>
-      </c>
-      <c r="B22" t="n">
-        <v>18820</v>
-      </c>
-      <c r="C22" t="n">
-        <v>8805</v>
-      </c>
-      <c r="D22" t="n">
-        <v>477</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5795</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1249</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1114</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1355</v>
-      </c>
-      <c r="I22" t="n">
-        <v>1604</v>
-      </c>
-      <c r="J22" t="n">
-        <v>506</v>
-      </c>
-      <c r="K22" t="n">
-        <v>769</v>
-      </c>
-      <c r="L22" t="n">
-        <v>557</v>
-      </c>
-      <c r="M22" t="n">
-        <v>409</v>
-      </c>
-      <c r="N22" t="n">
-        <v>2564</v>
-      </c>
-      <c r="O22" t="n">
-        <v>1068</v>
-      </c>
-      <c r="P22" t="n">
-        <v>1375</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>975</v>
-      </c>
-      <c r="R22" t="n">
-        <v>1236</v>
-      </c>
-      <c r="S22" t="n">
-        <v>657</v>
-      </c>
-      <c r="T22" t="n">
-        <v>457</v>
-      </c>
-      <c r="U22" t="n">
-        <v>901</v>
-      </c>
-      <c r="V22" t="n">
-        <v>5057</v>
-      </c>
-      <c r="W22" t="n">
-        <v>695</v>
-      </c>
-      <c r="X22" t="n">
-        <v>1501</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>608</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>58554</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>41883</v>
-      </c>
-      <c r="B23" t="n">
-        <v>18495</v>
-      </c>
-      <c r="C23" t="n">
-        <v>9712</v>
-      </c>
-      <c r="D23" t="n">
-        <v>517</v>
-      </c>
-      <c r="E23" t="n">
-        <v>5840</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1264</v>
-      </c>
-      <c r="G23" t="n">
-        <v>1148</v>
-      </c>
-      <c r="H23" t="n">
-        <v>1382</v>
-      </c>
-      <c r="I23" t="n">
-        <v>1618</v>
-      </c>
-      <c r="J23" t="n">
-        <v>525</v>
-      </c>
-      <c r="K23" t="n">
-        <v>714</v>
-      </c>
-      <c r="L23" t="n">
-        <v>614</v>
-      </c>
-      <c r="M23" t="n">
-        <v>349</v>
-      </c>
-      <c r="N23" t="n">
-        <v>2549</v>
-      </c>
-      <c r="O23" t="n">
-        <v>1097</v>
-      </c>
-      <c r="P23" t="n">
-        <v>1445</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>903</v>
-      </c>
-      <c r="R23" t="n">
-        <v>1258</v>
-      </c>
-      <c r="S23" t="n">
-        <v>660</v>
-      </c>
-      <c r="T23" t="n">
-        <v>512</v>
-      </c>
-      <c r="U23" t="n">
-        <v>1007</v>
-      </c>
-      <c r="V23" t="n">
-        <v>5173</v>
-      </c>
-      <c r="W23" t="n">
-        <v>676</v>
-      </c>
-      <c r="X23" t="n">
-        <v>1433</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>806</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>59697</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
-        <v>41913</v>
-      </c>
-      <c r="B24" t="n">
-        <v>17118</v>
-      </c>
-      <c r="C24" t="n">
-        <v>8826</v>
-      </c>
-      <c r="D24" t="n">
-        <v>439</v>
-      </c>
-      <c r="E24" t="n">
-        <v>5271</v>
-      </c>
-      <c r="F24" t="n">
-        <v>1178</v>
-      </c>
-      <c r="G24" t="n">
-        <v>998</v>
-      </c>
-      <c r="H24" t="n">
-        <v>1226</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1420</v>
-      </c>
-      <c r="J24" t="n">
-        <v>506</v>
-      </c>
-      <c r="K24" t="n">
-        <v>626</v>
-      </c>
-      <c r="L24" t="n">
-        <v>519</v>
-      </c>
-      <c r="M24" t="n">
-        <v>323</v>
-      </c>
-      <c r="N24" t="n">
-        <v>2232</v>
-      </c>
-      <c r="O24" t="n">
-        <v>965</v>
-      </c>
-      <c r="P24" t="n">
-        <v>1472</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>868</v>
-      </c>
-      <c r="R24" t="n">
-        <v>1207</v>
-      </c>
-      <c r="S24" t="n">
-        <v>640</v>
-      </c>
-      <c r="T24" t="n">
-        <v>493</v>
-      </c>
-      <c r="U24" t="n">
-        <v>958</v>
-      </c>
-      <c r="V24" t="n">
-        <v>4627</v>
-      </c>
-      <c r="W24" t="n">
-        <v>597</v>
-      </c>
-      <c r="X24" t="n">
-        <v>1437</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>753</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>54699</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>41944</v>
-      </c>
-      <c r="B25" t="n">
-        <v>12187</v>
-      </c>
-      <c r="C25" t="n">
-        <v>6905</v>
-      </c>
-      <c r="D25" t="n">
-        <v>287</v>
-      </c>
-      <c r="E25" t="n">
-        <v>3818</v>
-      </c>
-      <c r="F25" t="n">
-        <v>816</v>
-      </c>
-      <c r="G25" t="n">
-        <v>795</v>
-      </c>
-      <c r="H25" t="n">
-        <v>919</v>
-      </c>
-      <c r="I25" t="n">
-        <v>1050</v>
-      </c>
-      <c r="J25" t="n">
-        <v>402</v>
-      </c>
-      <c r="K25" t="n">
-        <v>541</v>
-      </c>
-      <c r="L25" t="n">
-        <v>375</v>
-      </c>
-      <c r="M25" t="n">
-        <v>187</v>
-      </c>
-      <c r="N25" t="n">
-        <v>1541</v>
-      </c>
-      <c r="O25" t="n">
-        <v>721</v>
-      </c>
-      <c r="P25" t="n">
-        <v>1071</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>677</v>
-      </c>
-      <c r="R25" t="n">
-        <v>892</v>
-      </c>
-      <c r="S25" t="n">
-        <v>398</v>
-      </c>
-      <c r="T25" t="n">
-        <v>351</v>
-      </c>
-      <c r="U25" t="n">
-        <v>712</v>
-      </c>
-      <c r="V25" t="n">
-        <v>3307</v>
-      </c>
-      <c r="W25" t="n">
-        <v>437</v>
-      </c>
-      <c r="X25" t="n">
-        <v>1111</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>568</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>40068</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>41974</v>
-      </c>
-      <c r="B26" t="n">
-        <v>9367</v>
-      </c>
-      <c r="C26" t="n">
-        <v>5843</v>
-      </c>
-      <c r="D26" t="n">
-        <v>224</v>
-      </c>
-      <c r="E26" t="n">
-        <v>2772</v>
-      </c>
-      <c r="F26" t="n">
-        <v>584</v>
-      </c>
-      <c r="G26" t="n">
-        <v>528</v>
-      </c>
-      <c r="H26" t="n">
-        <v>825</v>
-      </c>
-      <c r="I26" t="n">
-        <v>743</v>
-      </c>
-      <c r="J26" t="n">
-        <v>251</v>
-      </c>
-      <c r="K26" t="n">
-        <v>398</v>
-      </c>
-      <c r="L26" t="n">
-        <v>271</v>
-      </c>
-      <c r="M26" t="n">
-        <v>122</v>
-      </c>
-      <c r="N26" t="n">
-        <v>1068</v>
-      </c>
-      <c r="O26" t="n">
-        <v>443</v>
-      </c>
-      <c r="P26" t="n">
-        <v>847</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>532</v>
-      </c>
-      <c r="R26" t="n">
-        <v>781</v>
-      </c>
-      <c r="S26" t="n">
-        <v>253</v>
-      </c>
-      <c r="T26" t="n">
-        <v>253</v>
-      </c>
-      <c r="U26" t="n">
-        <v>584</v>
-      </c>
-      <c r="V26" t="n">
-        <v>2343</v>
-      </c>
-      <c r="W26" t="n">
-        <v>255</v>
-      </c>
-      <c r="X26" t="n">
-        <v>680</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>503</v>
-      </c>
-      <c r="Z26" t="n">
         <v>30470</v>
       </c>
     </row>

</xml_diff>